<commit_message>
wip: add Magic Card I
</commit_message>
<xml_diff>
--- a/ChemicalSummon/Assets/StreamingAssets/TranslatableSentence.xlsx
+++ b/ChemicalSummon/Assets/StreamingAssets/TranslatableSentence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="6"/>
+    <workbookView windowWidth="22368" windowHeight="9420" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="12" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="592">
   <si>
     <t>ScriptableObjectName</t>
   </si>
@@ -1599,6 +1599,42 @@
   </si>
   <si>
     <t>相手HP</t>
+  </si>
+  <si>
+    <t>Detonation</t>
+  </si>
+  <si>
+    <t>对一个热量释放1以上，剧烈度10以上的反应式发动。其释放全体爆炸伤害（热量释放量）*（剧烈度）。无法回收释放热量。</t>
+  </si>
+  <si>
+    <t>DustExplosion</t>
+  </si>
+  <si>
+    <t>对一个包含固体素材的，热量释放1以上，剧烈度5以上的反应式发动。其释放全体爆炸伤害（热量释放量）*（剧烈度）* 2。无法回收释放热量。</t>
+  </si>
+  <si>
+    <t>CompressedExplosion</t>
+  </si>
+  <si>
+    <t>对一个素材全是气体的，热量释放1以上，剧烈度5以上的反应式发动。其释放全体爆炸伤害（热量释放量）*（剧烈度）* 2。无法回收释放热量。</t>
+  </si>
+  <si>
+    <t>Melting</t>
+  </si>
+  <si>
+    <t>对一个热量释放5以上，剧烈度2以上的反应式发动。其对单个敌方卡牌升温至（热量释放量）*（剧烈度）* 20度。超过目标沸点时摧毁整个卡牌，超过目标熔点时弹回整个卡牌到敌方手牌。无法回收释放热量。</t>
+  </si>
+  <si>
+    <t>PaintProtection</t>
+  </si>
+  <si>
+    <t>这张卡放置在自己场上的卡牌叠上，禁止下面卡牌被融合素材指定。叠加数被任何原因更改时丢弃。</t>
+  </si>
+  <si>
+    <t>MetalRecycling</t>
+  </si>
+  <si>
+    <t>场上金属卡牌战损时发动。把它们加入自己手牌。被攻击方有优先发动权。</t>
   </si>
   <si>
     <t>ChangeCardBackground</t>
@@ -1774,10 +1810,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1789,7 +1825,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1803,29 +1869,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1833,7 +1877,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1847,9 +1898,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1863,9 +1914,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1879,24 +1936,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1918,17 +1960,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1941,7 +1977,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1953,7 +1995,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1965,61 +2133,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2031,73 +2145,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2113,18 +2161,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -2132,6 +2168,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2162,16 +2207,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2185,26 +2239,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2223,15 +2268,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2240,10 +2276,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2252,133 +2288,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2915,24 +2951,24 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" t="s">
-        <v>524</v>
+        <v>536</v>
       </c>
       <c r="C2" t="s">
-        <v>525</v>
+        <v>537</v>
       </c>
       <c r="D2" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="C3" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
       <c r="D3" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -2975,27 +3011,27 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" t="s">
-        <v>530</v>
+        <v>542</v>
       </c>
       <c r="B2" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="C2" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
       <c r="D2" t="s">
-        <v>533</v>
+        <v>545</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>534</v>
+        <v>546</v>
       </c>
       <c r="B3" t="s">
-        <v>535</v>
+        <v>547</v>
       </c>
       <c r="C3" t="s">
-        <v>536</v>
+        <v>548</v>
       </c>
       <c r="D3" t="s">
         <v>153</v>
@@ -3003,155 +3039,155 @@
     </row>
     <row r="4" customHeight="1" spans="1:4">
       <c r="A4" t="s">
-        <v>537</v>
+        <v>549</v>
       </c>
       <c r="B4" t="s">
-        <v>538</v>
+        <v>550</v>
       </c>
       <c r="C4" t="s">
-        <v>539</v>
+        <v>551</v>
       </c>
       <c r="D4" t="s">
-        <v>540</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:4">
       <c r="A5" t="s">
-        <v>541</v>
+        <v>553</v>
       </c>
       <c r="B5" t="s">
-        <v>542</v>
+        <v>554</v>
       </c>
       <c r="C5" t="s">
-        <v>543</v>
+        <v>555</v>
       </c>
       <c r="D5" t="s">
-        <v>544</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:4">
       <c r="A6" t="s">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="B6" t="s">
-        <v>546</v>
+        <v>558</v>
       </c>
       <c r="C6" t="s">
-        <v>547</v>
+        <v>559</v>
       </c>
       <c r="D6" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:4">
       <c r="A7" t="s">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="B7" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
       <c r="C7" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
       <c r="D7" t="s">
-        <v>552</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:4">
       <c r="A8" t="s">
-        <v>553</v>
+        <v>565</v>
       </c>
       <c r="B8" t="s">
-        <v>554</v>
+        <v>566</v>
       </c>
       <c r="C8" t="s">
-        <v>555</v>
+        <v>567</v>
       </c>
       <c r="D8" t="s">
-        <v>556</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:4">
       <c r="A9" t="s">
-        <v>557</v>
+        <v>569</v>
       </c>
       <c r="B9" t="s">
-        <v>558</v>
+        <v>570</v>
       </c>
       <c r="C9" t="s">
-        <v>559</v>
+        <v>571</v>
       </c>
       <c r="D9" t="s">
-        <v>560</v>
+        <v>572</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:4">
       <c r="A10" t="s">
-        <v>561</v>
+        <v>573</v>
       </c>
       <c r="C10" t="s">
-        <v>562</v>
+        <v>574</v>
       </c>
       <c r="D10" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:4">
       <c r="A11" t="s">
-        <v>564</v>
+        <v>576</v>
       </c>
       <c r="C11" t="s">
-        <v>565</v>
+        <v>577</v>
       </c>
       <c r="D11" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:4">
       <c r="A12" t="s">
-        <v>567</v>
+        <v>579</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>568</v>
+        <v>580</v>
       </c>
       <c r="C12" t="s">
-        <v>569</v>
+        <v>581</v>
       </c>
       <c r="D12" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:4">
       <c r="A13" t="s">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="C13" t="s">
-        <v>572</v>
+        <v>584</v>
       </c>
       <c r="D13" t="s">
-        <v>573</v>
+        <v>585</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:4">
       <c r="A14" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="C14" t="s">
-        <v>575</v>
+        <v>587</v>
       </c>
       <c r="D14" t="s">
-        <v>576</v>
+        <v>588</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:4">
       <c r="A15" t="s">
-        <v>577</v>
+        <v>589</v>
       </c>
       <c r="C15" t="s">
-        <v>578</v>
+        <v>590</v>
       </c>
       <c r="D15" t="s">
-        <v>579</v>
+        <v>591</v>
       </c>
     </row>
   </sheetData>
@@ -4869,8 +4905,8 @@
   <sheetPr/>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="3"/>
@@ -5040,10 +5076,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" outlineLevelCol="3"/>
@@ -5329,6 +5365,54 @@
         <v>523</v>
       </c>
     </row>
+    <row r="23" customHeight="1" spans="1:3">
+      <c r="A23" t="s">
+        <v>524</v>
+      </c>
+      <c r="C23" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:3">
+      <c r="A24" t="s">
+        <v>526</v>
+      </c>
+      <c r="C24" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:3">
+      <c r="A25" t="s">
+        <v>528</v>
+      </c>
+      <c r="C25" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:3">
+      <c r="A26" t="s">
+        <v>530</v>
+      </c>
+      <c r="C26" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:3">
+      <c r="A27" t="s">
+        <v>532</v>
+      </c>
+      <c r="C27" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="1:3">
+      <c r="A28" t="s">
+        <v>534</v>
+      </c>
+      <c r="C28" t="s">
+        <v>535</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>